<commit_message>
ADD: Calculations of risk assessment for public health from atmospheric air pollution (#3)
* add concentrations page

* fix naming

* upd header responsive

* add calculations riks page

* remake risks page & add 3 new calculations

* add info to form label

* remove redundant file
</commit_message>
<xml_diff>
--- a/lab1.xlsx
+++ b/lab1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Dima\Study\3year\5term\EM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395FC9E8-551F-45A0-BDE0-173948A7579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60952BA-94A2-4E51-98C5-7559FFF21088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
   </bookViews>
   <sheets>
     <sheet name="object" sheetId="1" r:id="rId1"/>
     <sheet name="pollution" sheetId="4" r:id="rId2"/>
     <sheet name="pollutant" sheetId="3" r:id="rId3"/>
+    <sheet name="pollutant_concentration" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -108,6 +109,12 @@
   </si>
   <si>
     <t>ПрАТ "Черкаське хімволокно"  ВП "Черкаська ТЕЦ"</t>
+  </si>
+  <si>
+    <t>concentration_value</t>
+  </si>
+  <si>
+    <t>Ангідрид сірчастий</t>
   </si>
 </sst>
 </file>
@@ -492,7 +499,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8028168-D1DD-4C4B-B4D0-7A72E2CEE3A7}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1429,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61FFF61-C7AB-456F-972E-F2ED96462917}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,6 +1539,243 @@
         <v>50</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECCF81F-484F-47F8-BBFF-4CFF976A40CF}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0.2767</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1.2917000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0.66669999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.83330000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>1.6667000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add losses calculator (#5)
* upd gitignore

* add losses calculator

* text formatting
</commit_message>
<xml_diff>
--- a/lab1.xlsx
+++ b/lab1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Dima\Study\3year\5term\EM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60952BA-94A2-4E51-98C5-7559FFF21088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB1C79C-E191-4FA2-9C32-3FB668CC2378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -1554,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECCF81F-484F-47F8-BBFF-4CFF976A40CF}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,10 +1693,10 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1704,10 +1704,10 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1715,10 +1715,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>0.65</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1726,10 +1726,10 @@
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1737,21 +1737,21 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>0.15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,10 +1759,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>1.5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1770,9 +1770,20 @@
         <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>0.28000000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add caclulating taxes for emissions
</commit_message>
<xml_diff>
--- a/lab1.xlsx
+++ b/lab1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Dima\Study\3year\5term\EM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB1C79C-E191-4FA2-9C32-3FB668CC2378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90687153-763A-4DE1-B80C-DD8F7F15D395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
   </bookViews>
   <sheets>
     <sheet name="object" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +115,66 @@
   </si>
   <si>
     <t>Ангідрид сірчастий</t>
+  </si>
+  <si>
+    <t>danger_class</t>
+  </si>
+  <si>
+    <t>tax_rate</t>
+  </si>
+  <si>
+    <t>Ацетон</t>
+  </si>
+  <si>
+    <t>Бенз(о)пірен</t>
+  </si>
+  <si>
+    <t>Бутилацетат</t>
+  </si>
+  <si>
+    <t>Ванадію п’ятиокис</t>
+  </si>
+  <si>
+    <t>9656,78</t>
+  </si>
+  <si>
+    <t>Водень хлористий</t>
+  </si>
+  <si>
+    <t>Вуглеводні</t>
+  </si>
+  <si>
+    <t>Газоподібні фтористі сполуки</t>
+  </si>
+  <si>
+    <t>Кадмію сполуки</t>
+  </si>
+  <si>
+    <t>Марганець та його сполуки</t>
+  </si>
+  <si>
+    <t>Нікель та його сполуки</t>
+  </si>
+  <si>
+    <t>Озон</t>
+  </si>
+  <si>
+    <t>Ртуть та її сполуки</t>
+  </si>
+  <si>
+    <t>Свинець та його сполуки</t>
+  </si>
+  <si>
+    <t>Сірковуглець</t>
+  </si>
+  <si>
+    <t>Спирт н-бутиловий</t>
+  </si>
+  <si>
+    <t>Стирол</t>
+  </si>
+  <si>
+    <t>Фенол</t>
   </si>
 </sst>
 </file>
@@ -138,8 +198,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -166,21 +226,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +588,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -533,7 +599,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -564,7 +630,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +715,7 @@
       <c r="A6">
         <v>2021</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
@@ -663,7 +729,7 @@
       <c r="A7">
         <v>2021</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
@@ -677,7 +743,7 @@
       <c r="A8">
         <v>2021</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
@@ -817,7 +883,7 @@
       <c r="A18">
         <v>2020</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
@@ -831,7 +897,7 @@
       <c r="A19">
         <v>2020</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C19" t="s">
@@ -845,7 +911,7 @@
       <c r="A20">
         <v>2020</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" t="s">
@@ -985,7 +1051,7 @@
       <c r="A30">
         <v>2019</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C30" t="s">
@@ -999,7 +1065,7 @@
       <c r="A31">
         <v>2019</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C31" t="s">
@@ -1013,7 +1079,7 @@
       <c r="A32">
         <v>2019</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C32" t="s">
@@ -1153,7 +1219,7 @@
       <c r="A42">
         <v>2018</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C42" t="s">
@@ -1167,7 +1233,7 @@
       <c r="A43">
         <v>2018</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C43" t="s">
@@ -1181,7 +1247,7 @@
       <c r="A44">
         <v>2018</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C44" t="s">
@@ -1321,7 +1387,7 @@
       <c r="A54">
         <v>2017</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C54" t="s">
@@ -1335,7 +1401,7 @@
       <c r="A55">
         <v>2017</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C55" t="s">
@@ -1349,7 +1415,7 @@
       <c r="A56">
         <v>2017</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C56" t="s">
@@ -1436,115 +1502,439 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61FFF61-C7AB-456F-972E-F2ED96462917}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8273.6299999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>482.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6373.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.5</v>
+      <c r="B12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>965.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3277278.63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>579.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6373.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>20376.22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="7">
+        <v>20376.22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>103816.62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>109127.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>109127.84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>8273.6299999999992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7">
+        <v>5376.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="D28" s="7">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>18799.080000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="7">
+        <v>11685.1</v>
       </c>
     </row>
   </sheetData>
@@ -1556,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECCF81F-484F-47F8-BBFF-4CFF976A40CF}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1579,7 +1969,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1590,7 +1980,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1601,7 +1991,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1612,7 +2002,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1623,7 +2013,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1634,7 +2024,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1645,7 +2035,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1656,7 +2046,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1667,7 +2057,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1678,7 +2068,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1689,7 +2079,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1700,7 +2090,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1711,7 +2101,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1722,7 +2112,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1733,7 +2123,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1744,7 +2134,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">

</xml_diff>

<commit_message>
Add taxes calculation (#6)
* add caclulating taxes for emissions

* upd db

* change default values

* add filtering

* remove redundant log
</commit_message>
<xml_diff>
--- a/lab1.xlsx
+++ b/lab1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Dima\Study\3year\5term\EM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB1C79C-E191-4FA2-9C32-3FB668CC2378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B875BA-D824-469A-951D-D2A5FB8BF87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
+    <workbookView minimized="1" xWindow="8880" yWindow="3075" windowWidth="13050" windowHeight="10350" activeTab="2" xr2:uid="{ED839A25-3011-423B-8600-4C4B93E29F33}"/>
   </bookViews>
   <sheets>
     <sheet name="object" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +115,66 @@
   </si>
   <si>
     <t>Ангідрид сірчастий</t>
+  </si>
+  <si>
+    <t>danger_class</t>
+  </si>
+  <si>
+    <t>tax_rate</t>
+  </si>
+  <si>
+    <t>Ацетон</t>
+  </si>
+  <si>
+    <t>Бенз(о)пірен</t>
+  </si>
+  <si>
+    <t>Бутилацетат</t>
+  </si>
+  <si>
+    <t>Ванадію п’ятиокис</t>
+  </si>
+  <si>
+    <t>9656,78</t>
+  </si>
+  <si>
+    <t>Водень хлористий</t>
+  </si>
+  <si>
+    <t>Вуглеводні</t>
+  </si>
+  <si>
+    <t>Газоподібні фтористі сполуки</t>
+  </si>
+  <si>
+    <t>Кадмію сполуки</t>
+  </si>
+  <si>
+    <t>Марганець та його сполуки</t>
+  </si>
+  <si>
+    <t>Нікель та його сполуки</t>
+  </si>
+  <si>
+    <t>Озон</t>
+  </si>
+  <si>
+    <t>Ртуть та її сполуки</t>
+  </si>
+  <si>
+    <t>Свинець та його сполуки</t>
+  </si>
+  <si>
+    <t>Сірковуглець</t>
+  </si>
+  <si>
+    <t>Спирт н-бутиловий</t>
+  </si>
+  <si>
+    <t>Стирол</t>
+  </si>
+  <si>
+    <t>Фенол</t>
   </si>
 </sst>
 </file>
@@ -138,8 +198,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -166,21 +226,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,7 +588,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -533,7 +599,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -564,7 +630,7 @@
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +715,7 @@
       <c r="A6">
         <v>2021</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
@@ -663,7 +729,7 @@
       <c r="A7">
         <v>2021</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
@@ -677,7 +743,7 @@
       <c r="A8">
         <v>2021</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
@@ -817,7 +883,7 @@
       <c r="A18">
         <v>2020</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
@@ -831,7 +897,7 @@
       <c r="A19">
         <v>2020</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C19" t="s">
@@ -845,7 +911,7 @@
       <c r="A20">
         <v>2020</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C20" t="s">
@@ -985,7 +1051,7 @@
       <c r="A30">
         <v>2019</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C30" t="s">
@@ -999,7 +1065,7 @@
       <c r="A31">
         <v>2019</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C31" t="s">
@@ -1013,7 +1079,7 @@
       <c r="A32">
         <v>2019</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C32" t="s">
@@ -1153,7 +1219,7 @@
       <c r="A42">
         <v>2018</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C42" t="s">
@@ -1167,7 +1233,7 @@
       <c r="A43">
         <v>2018</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C43" t="s">
@@ -1181,7 +1247,7 @@
       <c r="A44">
         <v>2018</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C44" t="s">
@@ -1321,7 +1387,7 @@
       <c r="A54">
         <v>2017</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C54" t="s">
@@ -1335,7 +1401,7 @@
       <c r="A55">
         <v>2017</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C55" t="s">
@@ -1349,7 +1415,7 @@
       <c r="A56">
         <v>2017</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C56" t="s">
@@ -1436,115 +1502,439 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61FFF61-C7AB-456F-972E-F2ED96462917}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8273.6299999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="2">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2">
+        <v>482.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6373.91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.5</v>
+      <c r="B12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>965.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="8">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3277278.63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="7">
+        <v>579.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6373.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>20376.22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="7">
+        <v>20376.22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>103816.62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>109127.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>109127.84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>8273.6299999999992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="7">
+        <v>5376.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="D28" s="7">
+        <v>2574.4299999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>18799.080000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="7">
+        <v>11685.1</v>
       </c>
     </row>
   </sheetData>
@@ -1556,7 +1946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECCF81F-484F-47F8-BBFF-4CFF976A40CF}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1579,7 +1969,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1590,7 +1980,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1601,7 +1991,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1612,7 +2002,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1623,7 +2013,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1634,7 +2024,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1645,7 +2035,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1656,7 +2046,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1667,7 +2057,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1678,7 +2068,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1689,7 +2079,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1700,7 +2090,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1711,7 +2101,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1722,7 +2112,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1733,7 +2123,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1744,7 +2134,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">

</xml_diff>